<commit_message>
added vc generate expp
</commit_message>
<xml_diff>
--- a/setups/vestibular chair/vPrime/lookup/vPrime Measurement.xlsx
+++ b/setups/vestibular chair/vPrime/lookup/vPrime Measurement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjheckman/Documents/Code/Gitlab/pbtoolbox/setups/vestibular chair/vPrime/lookup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF6D182-0740-6247-BE7E-ECF4702236AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C0E8E3-FB95-5146-BFDF-AB43AB93EDA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17060" yWindow="460" windowWidth="34140" windowHeight="27460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1349,7 +1349,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>